<commit_message>
Read images from folder
</commit_message>
<xml_diff>
--- a/coordenadas_fotos.xlsx
+++ b/coordenadas_fotos.xlsx
@@ -1,69 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanse77\Documents\Proyectos\GeoFotos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423E6DB1-41A0-4F8C-9267-3DEFA083D27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
-  <si>
-    <t>Nombre de la foto</t>
-  </si>
-  <si>
-    <t>Latitud</t>
-  </si>
-  <si>
-    <t>Longitud</t>
-  </si>
-  <si>
-    <t>20241214_143257.jpg</t>
-  </si>
-  <si>
-    <t>27°59'47.2″N</t>
-  </si>
-  <si>
-    <t>15°25'4.3″W</t>
-  </si>
-  <si>
-    <t>20241214_143533.jpg</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -78,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -402,51 +420,527 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.08984375" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre de la foto</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Latitud</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Longitud</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01.jpg</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>28°0'10.7″N</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>15°25'15.5″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>02.jpg</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>28°0'9.8″N</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>15°25'14.0″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>03.jpg</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>28°0'11.9″N</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>15°25'14.0″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>04.jpg</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>28°0'10.6″N</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>15°25'13.9″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05.jpg</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>28°0'10.6″N</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>15°25'13.9″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06.jpg</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>28°0'10.7″N</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>15°25'13.9″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>07.jpg</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>28°0'10.7″N</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>15°25'13.9″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>08.jpg</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>28°0'10.7″N</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>15°25'13.9″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>09.jpg</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>28°0'17.8″N</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>15°25'8.7″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10.jpg</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>28°0'17.3″N</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>15°25'10.1″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11.jpg</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>28°0'13.6″N</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>15°25'13.5″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12.jpg</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>28°0'18.5″N</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>15°25'14.4″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13.jpg</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>28°0'18.5″N</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>15°25'14.4″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14.jpg</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>28°0'14.9″N</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>15°25'14.3″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15.jpg</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>28°0'13.7″N</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>15°25'14.8″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16.jpg</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>28°0'13.7″N</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>15°25'14.6″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17.jpg</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>28°0'13.2″N</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>15°25'14.7″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18.jpg</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>28°0'13.2″N</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>15°25'14.6″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19.jpg</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>28°0'13.2″N</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>15°25'14.6″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20.jpg</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>28°0'13.2″N</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>15°25'14.6″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21.jpg</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>28°0'10.6″N</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>15°25'15.8″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22.jpg</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>28°0'10.6″N</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>15°25'15.8″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23.jpg</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>28°0'10.6″N</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>15°25'15.8″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24.jpg</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>28°0'12.4″N</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>15°25'14.4″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25.jpg</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>28°0'9.3″N</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>15°25'15.1″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26.jpg</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>28°0'9.3″N</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>15°25'15.1″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27.jpg</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>28°0'9.1″N</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>15°25'14.9″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28.jpg</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>28°0'10.1″N</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>15°25'15.4″W</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29.jpg</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>28°0'10.1″N</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>15°25'15.4″W</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>